<commit_message>
2024-01-08 update after structuring reviews
</commit_message>
<xml_diff>
--- a/src/data/raw/2024-01-03_review_papers.xlsx
+++ b/src/data/raw/2024-01-03_review_papers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lex/Workspace/phd-research-ucc/repositories/mrs-systematic-analysis/src/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716B334A-C3E8-0F4F-B4D2-447BBC3C83F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A9534F-F02C-614A-A20D-CF8FF8C72FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" activeTab="2" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="345">
   <si>
     <t>count</t>
   </si>
@@ -801,6 +801,282 @@
   </si>
   <si>
     <t>https://www.mendeley.com/</t>
+  </si>
+  <si>
+    <t>x121</t>
+  </si>
+  <si>
+    <t>Approaches to the Algorithmic Allocation of Public Resources: A Cross-disciplinary Review</t>
+  </si>
+  <si>
+    <t>Cross-disciplinary Review</t>
+  </si>
+  <si>
+    <t>To overview of the existing works in the field of public resource allocation and suggest guidance for the policy makers.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.48550/arXiv.2310.06475</t>
+  </si>
+  <si>
+    <t>Healthcare, disaster relief, organ transplantation, homelessness, welfare;</t>
+  </si>
+  <si>
+    <t>x128</t>
+  </si>
+  <si>
+    <t>Healthcare Operations Research and Management under Pandemics: a Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increase of social welfare from Healthcare System's point of view and public policymakers. </t>
+  </si>
+  <si>
+    <t>Papers on medical resource allocation under pandemic pressure.</t>
+  </si>
+  <si>
+    <t>https://optimization-online.org/2023/10/healthcare-operations-research-and-management-under-pandemics-a-review/</t>
+  </si>
+  <si>
+    <t>x333</t>
+  </si>
+  <si>
+    <t>The effect of overlapping surgical scheduling on operating theatre productivity: a narrative review</t>
+  </si>
+  <si>
+    <t>Narrative review</t>
+  </si>
+  <si>
+    <t>Analyse the effect of overlapping surgeries in scope of operation theatre time usage, ethics, training and safety asects.</t>
+  </si>
+  <si>
+    <t>COVID19 concequence &gt; 6 million patients in waiting list; Turnover = 15% = 72min in 8-h list;</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/anae.15797</t>
+  </si>
+  <si>
+    <t>x228</t>
+  </si>
+  <si>
+    <t>Operating room planning and scheduling: A literature review</t>
+  </si>
+  <si>
+    <t>Summarise the current trends in operating room planning and scheduling, and identify the directions for further research.</t>
+  </si>
+  <si>
+    <t>Data envelopment analysis (DEA);</t>
+  </si>
+  <si>
+    <t>https://isidore.co/CalibreLibrary/Garey,%20Michael%20R_/Computers%20and%20Intractability_%20A%20Guide%20to%20the%20Theory%20of%20NP-completeness%20(8927)/Computers%20and%20Intractability_%20A%20Guide%20to%20t%20-%20Garey,%20Michael%20R_.pdf</t>
+  </si>
+  <si>
+    <t>Problem complexities;</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1097/01.ta.0000220428.91423.78</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>SR0020BE11</t>
+  </si>
+  <si>
+    <t>SR0020BE12</t>
+  </si>
+  <si>
+    <t>SR0020BE13</t>
+  </si>
+  <si>
+    <t>SR0020BE14</t>
+  </si>
+  <si>
+    <t>SR0020BE15</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/ejores/v140y2002i3p541-561.html</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1097/00000539-200201000-00027</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1287/inte.32.2.63.57</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/WSC.2004.1371558</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1023/A:1019767900627</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10729-007-9011-1</t>
+  </si>
+  <si>
+    <t>SR0020BE16</t>
+  </si>
+  <si>
+    <t>SR0020BE17</t>
+  </si>
+  <si>
+    <t>SR0020BE18</t>
+  </si>
+  <si>
+    <t>Current Contents Connect</t>
+  </si>
+  <si>
+    <t>x235</t>
+  </si>
+  <si>
+    <t>Surgical demand scheduling: a review</t>
+  </si>
+  <si>
+    <t>Adminssions Scheduling and Control System (ASCS);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To address high meddical resouce cost, low healthcare facility utilisatation, and increasing demand for departments dependined on the surgical suite. </t>
+  </si>
+  <si>
+    <t>https://api.semanticscholar.org/CorpusID:46189607</t>
+  </si>
+  <si>
+    <t>x090</t>
+  </si>
+  <si>
+    <t>Assess the impact of modern technologies on healthcare.</t>
+  </si>
+  <si>
+    <t>A Review of Reinforcement Learning for Natural Language Processing, and Applications in Healthcare</t>
+  </si>
+  <si>
+    <t>General overview of ML tools in health care</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.48550/arXiv.2310.18354</t>
+  </si>
+  <si>
+    <t>SR0022US24</t>
+  </si>
+  <si>
+    <t>SR0022US25</t>
+  </si>
+  <si>
+    <t>SR0022US26</t>
+  </si>
+  <si>
+    <t>SR0022US27</t>
+  </si>
+  <si>
+    <t>A Comparative Study of Artificial Intelligence Applications in the Healthcare Sector</t>
+  </si>
+  <si>
+    <t>x101</t>
+  </si>
+  <si>
+    <t>Analyse the gaps between the practicies of AI in Bahrain and other countries around the world.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/978-981-99-6101-6_48</t>
+  </si>
+  <si>
+    <t>021IRSchedulingReview2020</t>
+  </si>
+  <si>
+    <t>Scientometric analysis</t>
+  </si>
+  <si>
+    <t>Systematic review, Meta-analysis (PRISMA)</t>
+  </si>
+  <si>
+    <t>A comprehensive review and analysis of operating room and surgery scheduling</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/15v0LOc7g5FOKGlNE7d0ZF2y1cbVMH6Ua/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11831-020-09432-2</t>
+  </si>
+  <si>
+    <t>Scheduling OT on the strategic, tactical, and operational levels of planning</t>
+  </si>
+  <si>
+    <t>SR0024IR20</t>
+  </si>
+  <si>
+    <t>Operating Room Turnover Time: Definitions and Future Research Needs</t>
+  </si>
+  <si>
+    <t>SR0025US19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of possible constrains for OT turnover time estimation </t>
+  </si>
+  <si>
+    <t>023USORTurnover2019</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1KDAaRtS-xTcMF-AO0klEMLyJ_jbFphUc/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177/1071181319631301</t>
+  </si>
+  <si>
+    <t>Healthcare scheduling in optimization context: a review</t>
+  </si>
+  <si>
+    <t>SR0026MY21</t>
+  </si>
+  <si>
+    <t>024MYSchedulingReview2021</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/15rAeJbb7ZCoS3GI_n0ZV-2UYJccbt137/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s12553-021-00547-5</t>
+  </si>
+  <si>
+    <t>Hard/soft constraints; Open-source db; Specialty statistics</t>
+  </si>
+  <si>
+    <t>032IRSchedulingReview2020</t>
+  </si>
+  <si>
+    <t>AR0027IR20</t>
+  </si>
+  <si>
+    <t>A state of the art review of intelligent scheduling</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10462-018-9667-6</t>
+  </si>
+  <si>
+    <t>044UGOpResInDevNatReview2023</t>
+  </si>
+  <si>
+    <t>The Application of Operations Research Information System Tools in Hospital Operations Management in Developing Nations: A Systematic Literature Review</t>
+  </si>
+  <si>
+    <t>SR0029UG23</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1uthkMoPEtUkt8wRKjF7zh3Y-hU4KVVH7/view</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.4314/udslj.v18i1.9</t>
+  </si>
+  <si>
+    <t>Comparison of OR&amp;M in developing countries and developed nations</t>
+  </si>
+  <si>
+    <t>Analyse OR&amp;M situation in developing nations of Africa</t>
+  </si>
+  <si>
+    <t>Pros and cons of metaheuristics</t>
+  </si>
+  <si>
+    <t>Survey intelligent scheduling systems</t>
+  </si>
+  <si>
+    <t>Extencive review</t>
   </si>
 </sst>
 </file>
@@ -883,7 +1159,7 @@
       <alignment horizontal="fill" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -904,12 +1180,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -917,7 +1194,7 @@
     <cellStyle name="Style 1" xfId="2" xr:uid="{AD703E83-2422-144D-99A8-2ADC57964367}"/>
     <cellStyle name="Style 2" xfId="3" xr:uid="{B9FF1B68-E23A-3C40-85DE-B173152847B9}"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -937,22 +1214,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -992,81 +1253,42 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1090,7 +1312,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1122,8 +1349,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}" name="Table1" displayName="Table1" ref="B2:U24" totalsRowShown="0">
-  <autoFilter ref="B2:U24" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}" name="Table1" displayName="Table1" ref="B2:U34" totalsRowShown="0">
+  <autoFilter ref="B2:U34" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{ED677BE4-361B-8D44-8CD6-F0AEEA011920}" name="count"/>
     <tableColumn id="2" xr3:uid="{FFD7AE9A-C033-3147-9E29-70AB2E220DDA}" name="pk"/>
@@ -1133,28 +1360,28 @@
     <tableColumn id="7" xr3:uid="{B5956E56-EA0C-C544-81E9-95D5F85516CE}" name="year"/>
     <tableColumn id="8" xr3:uid="{1D433107-5A8B-4B40-8584-1024473C053A}" name="type"/>
     <tableColumn id="9" xr3:uid="{28A710C7-54CD-BC4D-A29E-7C74FFEB5F42}" name="domain"/>
-    <tableColumn id="10" xr3:uid="{743D7D21-EF89-3A44-BB4E-7B8513684FD8}" name="grasp" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{E75B2E15-E73F-2743-8578-2D00366D3074}" name="group" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{DABBD7D1-C850-8F43-BA5A-928F99EA8729}" name="old_pk" dataDxfId="22"/>
-    <tableColumn id="13" xr3:uid="{E3DF3DD3-8A11-6E41-B2D8-7D4D4CC58F2B}" name="title" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{DBF169C0-2F63-7146-A2D1-70994280E63D}" name="method" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{743D7D21-EF89-3A44-BB4E-7B8513684FD8}" name="grasp" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{E75B2E15-E73F-2743-8578-2D00366D3074}" name="group" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{DABBD7D1-C850-8F43-BA5A-928F99EA8729}" name="old_pk" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{E3DF3DD3-8A11-6E41-B2D8-7D4D4CC58F2B}" name="title" dataDxfId="16"/>
+    <tableColumn id="14" xr3:uid="{DBF169C0-2F63-7146-A2D1-70994280E63D}" name="method" dataDxfId="15"/>
     <tableColumn id="17" xr3:uid="{5A2B4EE5-BF86-7042-97F7-E54C28D22FA9}" name="covid19"/>
-    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="12"/>
     <tableColumn id="19" xr3:uid="{E63FEC1A-8B57-1B47-AAEC-C5489A7E23BF}" name="coi"/>
-    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="20"/>
-    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="18"/>
-    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}" name="Table2" displayName="Table2" ref="B2:F37" totalsRowShown="0">
-  <autoFilter ref="B2:F37" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}" name="Table2" displayName="Table2" ref="B2:F46" totalsRowShown="0">
+  <autoFilter ref="B2:F46" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{E697A4C6-CB50-0449-AD63-6ACBEE53E663}" name="local_ref"/>
     <tableColumn id="3" xr3:uid="{53E59951-C7CE-0740-917C-0D957BB1897C}" name="ref_url"/>
     <tableColumn id="4" xr3:uid="{1E16B457-6000-4743-9439-9D6865E34250}" name="ref_comment"/>
@@ -1165,8 +1392,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A2C81E6-658C-CE40-B517-3E1650CBE932}" name="Table3" displayName="Table3" ref="B2:G35" totalsRowShown="0">
-  <autoFilter ref="B2:G35" xr:uid="{1A2C81E6-658C-CE40-B517-3E1650CBE932}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A2C81E6-658C-CE40-B517-3E1650CBE932}" name="Table3" displayName="Table3" ref="B2:G54" totalsRowShown="0">
+  <autoFilter ref="B2:G54" xr:uid="{1A2C81E6-658C-CE40-B517-3E1650CBE932}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{397B5144-7BE7-5040-A155-78DE0B051967}" name="pk"/>
     <tableColumn id="2" xr3:uid="{6EC61B08-E983-9A41-8626-3236E69BF335}" name="db_name"/>
@@ -1476,10 +1703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068F48D0-C0F6-0F48-8756-0A46C8000F25}">
-  <dimension ref="B1:U25"/>
+  <dimension ref="B2:U34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1493,24 +1720,21 @@
     <col min="7" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.1640625" customWidth="1"/>
-    <col min="11" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" style="16" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="51.5" customWidth="1"/>
     <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="33.83203125" style="16" customWidth="1"/>
-    <col min="21" max="21" width="33.1640625" customWidth="1"/>
+    <col min="20" max="20" width="33.83203125" customWidth="1"/>
+    <col min="21" max="21" width="36.83203125" customWidth="1"/>
     <col min="22" max="22" width="28.5" customWidth="1"/>
     <col min="23" max="23" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="M1"/>
-      <c r="T1"/>
-    </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
@@ -1607,16 +1831,18 @@
       <c r="L3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" t="s">
         <v>68</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" t="s">
         <v>185</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" s="3"/>
+      <c r="P3" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="Q3" t="s">
         <v>155</v>
       </c>
@@ -1626,7 +1852,7 @@
       <c r="S3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="13" t="s">
         <v>71</v>
       </c>
       <c r="U3" s="4" t="s">
@@ -1667,16 +1893,18 @@
       <c r="L4" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" t="s">
         <v>95</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" t="s">
         <v>96</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="Q4" t="s">
         <v>155</v>
       </c>
@@ -1686,7 +1914,7 @@
       <c r="S4" t="s">
         <v>220</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="13" t="s">
         <v>97</v>
       </c>
       <c r="U4" s="4" t="s">
@@ -1727,16 +1955,16 @@
       <c r="L5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" t="s">
         <v>119</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" t="s">
         <v>177</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5" s="17" t="s">
         <v>120</v>
       </c>
       <c r="Q5" t="s">
@@ -1748,7 +1976,7 @@
       <c r="S5" t="s">
         <v>176</v>
       </c>
-      <c r="T5" s="14" t="s">
+      <c r="T5" s="13" t="s">
         <v>145</v>
       </c>
       <c r="U5" s="4" t="s">
@@ -1789,16 +2017,18 @@
       <c r="L6" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" t="s">
         <v>146</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" t="s">
         <v>185</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="Q6" t="s">
         <v>155</v>
       </c>
@@ -1808,7 +2038,7 @@
       <c r="S6" t="s">
         <v>144</v>
       </c>
-      <c r="T6" s="14" t="s">
+      <c r="T6" s="13" t="s">
         <v>147</v>
       </c>
       <c r="U6" s="4" t="s">
@@ -1849,16 +2079,16 @@
       <c r="L7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" t="s">
         <v>151</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" t="s">
         <v>185</v>
       </c>
       <c r="O7">
         <v>1</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="17" t="s">
         <v>149</v>
       </c>
       <c r="Q7" t="s">
@@ -1870,7 +2100,7 @@
       <c r="S7" t="s">
         <v>148</v>
       </c>
-      <c r="T7" s="14" t="s">
+      <c r="T7" s="13" t="s">
         <v>152</v>
       </c>
       <c r="U7" s="4" t="s">
@@ -1911,16 +2141,16 @@
       <c r="L8" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M8" t="s">
         <v>157</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" t="s">
         <v>185</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="17" t="s">
         <v>159</v>
       </c>
       <c r="Q8" t="s">
@@ -1932,7 +2162,7 @@
       <c r="S8" t="s">
         <v>175</v>
       </c>
-      <c r="T8" s="14" t="s">
+      <c r="T8" s="13" t="s">
         <v>174</v>
       </c>
       <c r="U8" s="4" t="s">
@@ -1973,16 +2203,18 @@
       <c r="L9" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" t="s">
         <v>183</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="N9" t="s">
         <v>185</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="Q9" t="s">
         <v>154</v>
       </c>
@@ -1992,7 +2224,7 @@
       <c r="S9" t="s">
         <v>181</v>
       </c>
-      <c r="T9" s="15" t="s">
+      <c r="T9" s="14" t="s">
         <v>182</v>
       </c>
       <c r="U9" s="4" t="s">
@@ -2033,16 +2265,16 @@
       <c r="L10" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" t="s">
         <v>188</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="N10" t="s">
         <v>75</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="17" t="s">
         <v>190</v>
       </c>
       <c r="Q10" t="s">
@@ -2054,7 +2286,7 @@
       <c r="S10" t="s">
         <v>191</v>
       </c>
-      <c r="T10" s="15" t="s">
+      <c r="T10" s="14" t="s">
         <v>192</v>
       </c>
       <c r="U10" s="4" t="s">
@@ -2095,16 +2327,16 @@
       <c r="L11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" t="s">
         <v>193</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="N11" t="s">
         <v>197</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="P11" s="17" t="s">
         <v>196</v>
       </c>
       <c r="Q11" t="s">
@@ -2116,7 +2348,7 @@
       <c r="S11" t="s">
         <v>195</v>
       </c>
-      <c r="T11" s="15" t="s">
+      <c r="T11" s="14" t="s">
         <v>198</v>
       </c>
       <c r="U11" s="4" t="s">
@@ -2157,16 +2389,16 @@
       <c r="L12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" t="s">
         <v>199</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="N12" t="s">
         <v>201</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" s="17" t="s">
         <v>202</v>
       </c>
       <c r="Q12" t="s">
@@ -2178,7 +2410,7 @@
       <c r="S12" t="s">
         <v>204</v>
       </c>
-      <c r="T12" s="15" t="s">
+      <c r="T12" s="14" t="s">
         <v>203</v>
       </c>
       <c r="U12" s="4" t="s">
@@ -2219,16 +2451,18 @@
       <c r="L13" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" t="s">
         <v>214</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="N13" t="s">
         <v>185</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="P13" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="Q13" t="s">
         <v>154</v>
       </c>
@@ -2238,7 +2472,7 @@
       <c r="S13" t="s">
         <v>215</v>
       </c>
-      <c r="T13" s="15" t="s">
+      <c r="T13" s="14" t="s">
         <v>216</v>
       </c>
       <c r="U13" s="4" t="s">
@@ -2279,16 +2513,18 @@
       <c r="L14" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="M14" t="s">
         <v>218</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="N14" t="s">
         <v>185</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="3"/>
+      <c r="P14" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="Q14" t="s">
         <v>154</v>
       </c>
@@ -2298,7 +2534,7 @@
       <c r="S14" t="s">
         <v>219</v>
       </c>
-      <c r="T14" s="15" t="s">
+      <c r="T14" s="14" t="s">
         <v>108</v>
       </c>
       <c r="U14" s="4" t="s">
@@ -2339,16 +2575,18 @@
       <c r="L15" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="M15" s="16" t="s">
+      <c r="M15" t="s">
         <v>223</v>
       </c>
-      <c r="N15" s="12" t="s">
+      <c r="N15" t="s">
         <v>185</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15" s="3"/>
+      <c r="P15" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="Q15" t="s">
         <v>155</v>
       </c>
@@ -2358,7 +2596,7 @@
       <c r="S15" t="s">
         <v>224</v>
       </c>
-      <c r="T15" s="15" t="s">
+      <c r="T15" s="14" t="s">
         <v>225</v>
       </c>
       <c r="U15" s="4" t="s">
@@ -2399,16 +2637,16 @@
       <c r="L16" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="M16" t="s">
         <v>231</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N16" t="s">
         <v>185</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" s="17" t="s">
         <v>233</v>
       </c>
       <c r="Q16" t="s">
@@ -2420,7 +2658,7 @@
       <c r="S16" t="s">
         <v>234</v>
       </c>
-      <c r="T16" s="15" t="s">
+      <c r="T16" s="14" t="s">
         <v>232</v>
       </c>
       <c r="U16" s="4" t="s">
@@ -2461,16 +2699,16 @@
       <c r="L17" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" t="s">
         <v>244</v>
       </c>
-      <c r="N17" s="12" t="s">
+      <c r="N17" t="s">
         <v>185</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="P17" s="17" t="s">
         <v>247</v>
       </c>
       <c r="Q17" t="s">
@@ -2482,7 +2720,7 @@
       <c r="S17" t="s">
         <v>245</v>
       </c>
-      <c r="T17" s="15" t="s">
+      <c r="T17" s="14" t="s">
         <v>246</v>
       </c>
       <c r="U17" s="4" t="s">
@@ -2496,11 +2734,57 @@
       <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="2"/>
-      <c r="N18" s="17"/>
-      <c r="P18" s="3"/>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18">
+        <v>2023</v>
+      </c>
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="K18" s="5">
+        <v>6</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M18" t="s">
+        <v>254</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>155</v>
+      </c>
+      <c r="R18" t="s">
+        <v>155</v>
+      </c>
+      <c r="S18" t="s">
+        <v>258</v>
+      </c>
+      <c r="T18" s="14" t="s">
+        <v>257</v>
+      </c>
       <c r="U18" s="4" t="s">
         <v>69</v>
       </c>
@@ -2512,11 +2796,57 @@
       <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="2"/>
-      <c r="N19" s="17"/>
-      <c r="P19" s="3"/>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19">
+        <v>2023</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K19" s="5">
+        <v>6</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M19" t="s">
+        <v>260</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>155</v>
+      </c>
+      <c r="R19" t="s">
+        <v>187</v>
+      </c>
+      <c r="S19" t="s">
+        <v>262</v>
+      </c>
+      <c r="T19" s="14" t="s">
+        <v>263</v>
+      </c>
       <c r="U19" s="4" t="s">
         <v>69</v>
       </c>
@@ -2528,11 +2858,57 @@
       <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="2"/>
-      <c r="N20" s="17"/>
-      <c r="P20" s="3"/>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20">
+        <v>2022</v>
+      </c>
+      <c r="H20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="K20" s="5">
+        <v>6</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="M20" t="s">
+        <v>265</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>154</v>
+      </c>
+      <c r="R20" t="s">
+        <v>156</v>
+      </c>
+      <c r="S20" t="s">
+        <v>268</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>269</v>
+      </c>
       <c r="U20" s="4" t="s">
         <v>69</v>
       </c>
@@ -2544,11 +2920,57 @@
       <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="2"/>
-      <c r="N21" s="17"/>
-      <c r="P21" s="3"/>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <v>2010</v>
+      </c>
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="K21" s="5">
+        <v>6</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="M21" t="s">
+        <v>271</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>155</v>
+      </c>
+      <c r="R21" t="s">
+        <v>155</v>
+      </c>
+      <c r="S21" t="s">
+        <v>273</v>
+      </c>
+      <c r="T21" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="U21" s="4" t="s">
         <v>69</v>
       </c>
@@ -2560,11 +2982,57 @@
       <c r="C22" t="s">
         <v>61</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="2"/>
-      <c r="N22" s="17"/>
-      <c r="P22" s="3"/>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22">
+        <v>1978</v>
+      </c>
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="K22" s="5">
+        <v>6</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="M22" t="s">
+        <v>294</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>155</v>
+      </c>
+      <c r="R22" t="s">
+        <v>155</v>
+      </c>
+      <c r="S22" t="s">
+        <v>295</v>
+      </c>
+      <c r="T22" s="14" t="s">
+        <v>297</v>
+      </c>
       <c r="U22" s="4" t="s">
         <v>69</v>
       </c>
@@ -2576,11 +3044,57 @@
       <c r="C23" t="s">
         <v>62</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="2"/>
-      <c r="N23" s="17"/>
-      <c r="P23" s="3"/>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23">
+        <v>2023</v>
+      </c>
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="K23" s="5">
+        <v>6</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="M23" t="s">
+        <v>300</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>153</v>
+      </c>
+      <c r="R23" t="s">
+        <v>186</v>
+      </c>
+      <c r="S23" t="s">
+        <v>301</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>302</v>
+      </c>
       <c r="U23" s="4" t="s">
         <v>69</v>
       </c>
@@ -2592,26 +3106,450 @@
       <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="2"/>
-      <c r="N24" s="17"/>
-      <c r="P24" s="3"/>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <v>2023</v>
+      </c>
+      <c r="H24" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" t="s">
+        <v>248</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="M24" t="s">
+        <v>307</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>155</v>
+      </c>
+      <c r="R24" t="s">
+        <v>155</v>
+      </c>
+      <c r="S24" t="s">
+        <v>224</v>
+      </c>
+      <c r="T24" s="14" t="s">
+        <v>310</v>
+      </c>
       <c r="U24" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="R25" s="3"/>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25">
+        <v>2020</v>
+      </c>
+      <c r="H25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="K25" s="5">
+        <v>2</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="M25" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>153</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="S25" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="T25" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="U25" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>320</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26">
+        <v>2019</v>
+      </c>
+      <c r="H26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" t="s">
+        <v>65</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="K26" s="5">
+        <v>2</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>155</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="S26" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="T26" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="U26" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>326</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27">
+        <v>2021</v>
+      </c>
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="K27" s="5">
+        <v>2</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>155</v>
+      </c>
+      <c r="R27" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="S27" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="T27" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="U27" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>332</v>
+      </c>
+      <c r="E28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28">
+        <v>2020</v>
+      </c>
+      <c r="H28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K28" s="5">
+        <v>3</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>155</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="S28" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="T28" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="U28" s="3"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>337</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29">
+        <v>2023</v>
+      </c>
+      <c r="H29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29" t="s">
+        <v>66</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K29" s="5">
+        <v>4</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="M29" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>155</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="S29" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="T29" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="U29" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" t="s">
+        <v>38</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="15"/>
+      <c r="P30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="3"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" t="s">
+        <v>38</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="15"/>
+      <c r="P31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="18"/>
+      <c r="U31" s="3"/>
+    </row>
+    <row r="33" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J33" s="1"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="15"/>
+      <c r="P33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="18"/>
+      <c r="U33" s="3"/>
+    </row>
+    <row r="34" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J34" s="1"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="15"/>
+      <c r="P34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
+      <c r="U34" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E24">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="E33:E34 E3:E31">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J24">
-    <cfRule type="dataBar" priority="17">
+  <conditionalFormatting sqref="I33:I34 I3:I31">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>"None"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33:J34 J3:J31">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2624,37 +3562,37 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O24">
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+  <conditionalFormatting sqref="N33:N34 N3:N31">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
+      <formula>"not specified"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"not specified"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O33:O34 O3:O31">
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:R24">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
+  <conditionalFormatting sqref="Q33:R34 Q3:R31">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">
       <formula>"Not mentioned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"not mentioned"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N24">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">
-      <formula>"not specified"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="P33:P34 P3:P31">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"not specified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I24">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"None"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B24" xr:uid="{A8AF43FC-C864-0442-BE4D-1BD3B99797F0}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B34 B3:B31" xr:uid="{A8AF43FC-C864-0442-BE4D-1BD3B99797F0}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D24" xr:uid="{DE81B6F3-8CEE-BE43-8C07-AF5DC780196D}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D33:D34 D3:D31" xr:uid="{DE81B6F3-8CEE-BE43-8C07-AF5DC780196D}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
@@ -2683,10 +3621,26 @@
     <hyperlink ref="T15" r:id="rId21" xr:uid="{CA3CFD41-4343-BF47-BDBD-E6941AB200A3}"/>
     <hyperlink ref="T16" r:id="rId22" xr:uid="{DD2FF52B-8D35-A44E-B0ED-45D5D61D0F07}"/>
     <hyperlink ref="T17" r:id="rId23" xr:uid="{51F7187F-5358-2849-8472-7C3E4E859657}"/>
+    <hyperlink ref="T18" r:id="rId24" xr:uid="{029ED567-C070-B34C-B6D7-D80577E39992}"/>
+    <hyperlink ref="T19" r:id="rId25" xr:uid="{A7329540-65FD-1849-84D2-9244B1BD561A}"/>
+    <hyperlink ref="T20" r:id="rId26" xr:uid="{6A99BFD4-BAB3-7A45-9A88-C5E85FDFF0C8}"/>
+    <hyperlink ref="T21" r:id="rId27" xr:uid="{04A2209A-C01E-4345-AC8F-8B28470D961F}"/>
+    <hyperlink ref="T22" r:id="rId28" xr:uid="{8C5C6103-3A84-CD4B-B0E4-AFB6CBE6268E}"/>
+    <hyperlink ref="T23" r:id="rId29" xr:uid="{4E874567-21A8-234D-ABB7-163AB8D80682}"/>
+    <hyperlink ref="T24" r:id="rId30" xr:uid="{D8F31D70-FEFF-F846-A7B5-58B69D6348ED}"/>
+    <hyperlink ref="U25" r:id="rId31" xr:uid="{2EE5E883-FCE4-8C42-94BC-7A922E62DC65}"/>
+    <hyperlink ref="T25" r:id="rId32" xr:uid="{B475C20A-2E9C-0C4D-B7B7-02C4E5864019}"/>
+    <hyperlink ref="U26" r:id="rId33" xr:uid="{A9EF7319-5B1C-D74E-A561-0DD548530505}"/>
+    <hyperlink ref="T26" r:id="rId34" xr:uid="{CD1BA2B8-9D7A-E549-8FAE-C43DAA1D1D10}"/>
+    <hyperlink ref="U27" r:id="rId35" xr:uid="{51AB83C7-1D02-3D46-8BB5-79D8553CEE32}"/>
+    <hyperlink ref="T27" r:id="rId36" xr:uid="{E9B28FC3-0E80-7645-879C-F52BF29A88F8}"/>
+    <hyperlink ref="T28" r:id="rId37" xr:uid="{A89A9514-5C6D-C64F-8A1B-9355F32E3BF0}"/>
+    <hyperlink ref="U29" r:id="rId38" xr:uid="{4C1F5746-7BAC-484E-A22B-6A77AC8DA912}"/>
+    <hyperlink ref="T29" r:id="rId39" xr:uid="{6E76C6C8-A0B3-A947-8EC9-08753C886A4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId40"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -2704,7 +3658,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J3:J24</xm:sqref>
+          <xm:sqref>J33:J34 J3:J31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2714,43 +3668,43 @@
           <x14:formula1>
             <xm:f>factors!$C$3:$C$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F24</xm:sqref>
+          <xm:sqref>F33:F34 F3:F31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{497BC3DD-CEC8-2747-860E-683E9AB8EA62}">
           <x14:formula1>
             <xm:f>factors!$D$3:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E24</xm:sqref>
+          <xm:sqref>E33:E34 E3:E31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F2C01858-56B7-724A-B24C-A857D3030B5A}">
           <x14:formula1>
             <xm:f>factors!$E$3:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H24</xm:sqref>
+          <xm:sqref>H33:H34 H3:H31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{566B1144-F99A-C245-8189-04C656B42A78}">
           <x14:formula1>
             <xm:f>factors!$F$3:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I24</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBAE5E32-2C54-BA45-86E5-09D8CE417A28}">
-          <x14:formula1>
-            <xm:f>factors!$G$3:$G$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>N3:N24</xm:sqref>
+          <xm:sqref>I33:I34 I3:I31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1AA26AE0-EDAD-8C47-ACEB-3F6AE8EEE028}">
           <x14:formula1>
             <xm:f>factors!$K$3:$K$9</xm:f>
           </x14:formula1>
-          <xm:sqref>Q3:Q24</xm:sqref>
+          <xm:sqref>Q33:Q34 Q3:Q31</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{23A70AE2-6E88-4942-88A7-3AD2C2C96B60}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBAE5E32-2C54-BA45-86E5-09D8CE417A28}">
           <x14:formula1>
-            <xm:f>factors!$L$3:$L$11</xm:f>
+            <xm:f>factors!$G$3:$G$21</xm:f>
           </x14:formula1>
-          <xm:sqref>R3:R24</xm:sqref>
+          <xm:sqref>N33:N34 N3:N31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{745EE373-4BD2-1042-AADC-7EDFB98FA266}">
+          <x14:formula1>
+            <xm:f>factors!$L$3:$L$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>R33:R34 R3:R31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2760,10 +3714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7254ACE7-56C6-5040-ABFE-788EED7DE7C7}">
-  <dimension ref="B2:I37"/>
+  <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3112,7 +4066,7 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="12" t="s">
+      <c r="B32" t="s">
         <v>51</v>
       </c>
       <c r="C32">
@@ -3127,8 +4081,7 @@
       <c r="I32" s="11"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="12"/>
-      <c r="I33" s="13"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
@@ -3143,7 +4096,7 @@
       <c r="E34" t="s">
         <v>241</v>
       </c>
-      <c r="I34" s="13"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
@@ -3159,11 +4112,123 @@
         <v>242</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="12"/>
-    </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="12"/>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>55</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E37" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E38" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E39" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41">
+        <v>14</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E41" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="C42">
+        <v>53</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E42" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="C43">
+        <v>64</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E43" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C44">
+        <v>109</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3196,10 +4261,18 @@
     <hyperlink ref="D31" r:id="rId26" xr:uid="{D5FD0FEA-0E5D-B74A-9920-3B8F9A04A4BD}"/>
     <hyperlink ref="D34" r:id="rId27" xr:uid="{CB62A20C-2A06-3F49-B0ED-47D641C90CC2}"/>
     <hyperlink ref="D35" r:id="rId28" xr:uid="{55A3C2F6-C9A4-E54D-8B07-E30F20F15CD0}"/>
+    <hyperlink ref="D37" r:id="rId29" xr:uid="{E01B0CF2-6BFE-D345-B7D6-C0B9C0750721}"/>
+    <hyperlink ref="D38" r:id="rId30" xr:uid="{A0EDAFCC-32C8-C54B-B95A-3FCD6EB27A4E}"/>
+    <hyperlink ref="D39" r:id="rId31" xr:uid="{B7A98387-F885-6A4D-8AB6-D1E499508E31}"/>
+    <hyperlink ref="D40" r:id="rId32" xr:uid="{129B8CCF-B618-704C-A4B0-F7AB8A3E1964}"/>
+    <hyperlink ref="D41" r:id="rId33" xr:uid="{54C82C25-7642-0E43-A781-CA0CA8B784A7}"/>
+    <hyperlink ref="D42" r:id="rId34" xr:uid="{B11A1E93-5864-B843-9CB5-557F0F8E5E36}"/>
+    <hyperlink ref="D43" r:id="rId35" xr:uid="{471C162F-9F71-734A-9014-76CD511D05CB}"/>
+    <hyperlink ref="D44" r:id="rId36" xr:uid="{54A17B45-9CAF-704A-92DF-92CF3F3F7D13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId37"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -3218,10 +4291,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCB2E3E-28B4-564E-8BB1-3B4DB94D469B}">
-  <dimension ref="B2:I35"/>
+  <dimension ref="B2:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3436,7 +4509,7 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
+      <c r="B19" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -3453,7 +4526,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
+      <c r="B20" t="s">
         <v>51</v>
       </c>
       <c r="C20" t="s">
@@ -3465,7 +4538,7 @@
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="12" t="s">
+      <c r="B21" t="s">
         <v>51</v>
       </c>
       <c r="C21" t="s">
@@ -3477,7 +4550,7 @@
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="12" t="s">
+      <c r="B22" t="s">
         <v>51</v>
       </c>
       <c r="C22" t="s">
@@ -3494,11 +4567,10 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="12"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
+      <c r="B24" t="s">
         <v>53</v>
       </c>
       <c r="C24" t="s">
@@ -3510,7 +4582,7 @@
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="12" t="s">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
       <c r="C25" t="s">
@@ -3522,7 +4594,7 @@
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="12" t="s">
+      <c r="B26" t="s">
         <v>53</v>
       </c>
       <c r="C26" t="s">
@@ -3534,7 +4606,7 @@
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="12" t="s">
+      <c r="B27" t="s">
         <v>53</v>
       </c>
       <c r="C27" t="s">
@@ -3626,9 +4698,160 @@
         <v>252</v>
       </c>
     </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="C38" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C39" t="s">
+        <v>292</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" t="s">
+        <v>226</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>303</v>
+      </c>
+      <c r="C43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>304</v>
+      </c>
+      <c r="C44" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>305</v>
+      </c>
+      <c r="C45" t="s">
+        <v>162</v>
+      </c>
+      <c r="D45" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>306</v>
+      </c>
+      <c r="C46" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>318</v>
+      </c>
+      <c r="C48" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="6"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C3:C35">
+  <conditionalFormatting sqref="C3:C54">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>COUNTIF($C$3:$C3,$C3)&gt;1</formula>
     </cfRule>
@@ -3651,10 +4874,11 @@
     <hyperlink ref="F31" r:id="rId15" xr:uid="{0CA930B9-8A70-0748-B269-CB8C06557907}"/>
     <hyperlink ref="F34" r:id="rId16" xr:uid="{66A76C66-F913-B340-BEDA-147F8159ABBC}"/>
     <hyperlink ref="F35" r:id="rId17" xr:uid="{4B98ED98-7408-6042-B386-64B2B53F986D}"/>
+    <hyperlink ref="F39" r:id="rId18" xr:uid="{47324C33-A3FB-8A49-B2B2-4760A3B99BAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -3663,7 +4887,7 @@
           <x14:formula1>
             <xm:f>factors!$I$3:$I$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D35</xm:sqref>
+          <xm:sqref>D3:D54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A4B89F4-DB21-124C-8D10-52A35A151DF7}">
           <x14:formula1>
@@ -3789,10 +5013,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8227E6-DB79-7241-B7AF-4C424F805AD9}">
-  <dimension ref="B2:L11"/>
+  <dimension ref="B2:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3991,12 +5215,40 @@
         <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>185</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024-01-10 start setuping the workflow for summaries
</commit_message>
<xml_diff>
--- a/src/data/raw/2024-01-03_review_papers.xlsx
+++ b/src/data/raw/2024-01-03_review_papers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lex/Workspace/phd-research-ucc/repositories/mrs-systematic-analysis/src/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F35F60E-01B3-8D40-AADA-8C81A96BAF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A9B8D2-E3BA-1347-A137-1B7A2BF620B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" xr2:uid="{42FB9FC8-AC2E-C945-8759-9355EAD5812E}"/>
   </bookViews>
   <sheets>
     <sheet name="papers" sheetId="1" r:id="rId1"/>
@@ -1159,7 +1159,7 @@
       <alignment horizontal="fill" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1184,9 +1184,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1207,13 +1204,9 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1227,9 +1220,13 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1278,19 +1275,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1307,6 +1291,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1351,6 +1348,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}" name="Table1" displayName="Table1" ref="B2:U34" totalsRowShown="0">
   <autoFilter ref="B2:U34" xr:uid="{02E67EF5-CF56-8A46-AAD1-7367959AC624}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:U34">
+    <sortCondition ref="B2:B34"/>
+  </sortState>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{ED677BE4-361B-8D44-8CD6-F0AEEA011920}" name="count"/>
     <tableColumn id="2" xr3:uid="{FFD7AE9A-C033-3147-9E29-70AB2E220DDA}" name="pk"/>
@@ -1366,12 +1366,12 @@
     <tableColumn id="13" xr3:uid="{E3DF3DD3-8A11-6E41-B2D8-7D4D4CC58F2B}" name="title" dataDxfId="16"/>
     <tableColumn id="14" xr3:uid="{DBF169C0-2F63-7146-A2D1-70994280E63D}" name="method" dataDxfId="15"/>
     <tableColumn id="17" xr3:uid="{5A2B4EE5-BF86-7042-97F7-E54C28D22FA9}" name="covid19"/>
-    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="12"/>
+    <tableColumn id="18" xr3:uid="{50337C7A-AEB8-6A41-9E80-81EE1EE770BC}" name="objectives" dataDxfId="14"/>
     <tableColumn id="19" xr3:uid="{E63FEC1A-8B57-1B47-AAEC-C5489A7E23BF}" name="coi"/>
-    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="14"/>
-    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="10"/>
-    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="9"/>
+    <tableColumn id="20" xr3:uid="{FAB4274B-32D5-714B-AEC0-065807D96185}" name="funding" dataDxfId="13"/>
+    <tableColumn id="21" xr3:uid="{329430AD-233F-7844-8FD3-986B1229B338}" name="comment" dataDxfId="12"/>
+    <tableColumn id="22" xr3:uid="{7F68878B-5789-5D4B-88C5-2071869281AC}" name="url" dataDxfId="11"/>
+    <tableColumn id="23" xr3:uid="{46B5E7B4-3D1C-CD4B-8B57-EAB7415DFC0D}" name="review_url" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1381,7 +1381,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}" name="Table2" displayName="Table2" ref="B2:F46" totalsRowShown="0">
   <autoFilter ref="B2:F46" xr:uid="{07674F2D-48E4-6445-B114-EAC6E0A8140D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{F57613C8-BD69-D744-AEED-50188C65CB98}" name="pk" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{E697A4C6-CB50-0449-AD63-6ACBEE53E663}" name="local_ref"/>
     <tableColumn id="3" xr3:uid="{53E59951-C7CE-0740-917C-0D957BB1897C}" name="ref_url"/>
     <tableColumn id="4" xr3:uid="{1E16B457-6000-4743-9439-9D6865E34250}" name="ref_comment"/>
@@ -1706,7 +1706,7 @@
   <dimension ref="B2:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1722,7 +1722,7 @@
     <col min="10" max="10" width="13.1640625" customWidth="1"/>
     <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" customWidth="1"/>
+    <col min="13" max="13" width="39" customWidth="1"/>
     <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="51.5" customWidth="1"/>
@@ -1840,7 +1840,7 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" t="s">
         <v>185</v>
       </c>
       <c r="Q3" t="s">
@@ -1902,7 +1902,7 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="P4" t="s">
         <v>185</v>
       </c>
       <c r="Q4" t="s">
@@ -1964,7 +1964,7 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" t="s">
         <v>120</v>
       </c>
       <c r="Q5" t="s">
@@ -2026,7 +2026,7 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="P6" t="s">
         <v>185</v>
       </c>
       <c r="Q6" t="s">
@@ -2088,7 +2088,7 @@
       <c r="O7">
         <v>1</v>
       </c>
-      <c r="P7" s="17" t="s">
+      <c r="P7" t="s">
         <v>149</v>
       </c>
       <c r="Q7" t="s">
@@ -2150,7 +2150,7 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8" s="17" t="s">
+      <c r="P8" t="s">
         <v>159</v>
       </c>
       <c r="Q8" t="s">
@@ -2212,7 +2212,7 @@
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="P9" t="s">
         <v>185</v>
       </c>
       <c r="Q9" t="s">
@@ -2274,7 +2274,7 @@
       <c r="O10">
         <v>1</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="P10" t="s">
         <v>190</v>
       </c>
       <c r="Q10" t="s">
@@ -2336,7 +2336,7 @@
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" t="s">
         <v>196</v>
       </c>
       <c r="Q11" t="s">
@@ -2398,7 +2398,7 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="P12" t="s">
         <v>202</v>
       </c>
       <c r="Q12" t="s">
@@ -2460,7 +2460,7 @@
       <c r="O13">
         <v>1</v>
       </c>
-      <c r="P13" s="17" t="s">
+      <c r="P13" t="s">
         <v>185</v>
       </c>
       <c r="Q13" t="s">
@@ -2522,7 +2522,7 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="17" t="s">
+      <c r="P14" t="s">
         <v>185</v>
       </c>
       <c r="Q14" t="s">
@@ -2584,7 +2584,7 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15" s="17" t="s">
+      <c r="P15" t="s">
         <v>185</v>
       </c>
       <c r="Q15" t="s">
@@ -2646,7 +2646,7 @@
       <c r="O16">
         <v>1</v>
       </c>
-      <c r="P16" s="17" t="s">
+      <c r="P16" t="s">
         <v>233</v>
       </c>
       <c r="Q16" t="s">
@@ -2708,7 +2708,7 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17" s="17" t="s">
+      <c r="P17" t="s">
         <v>247</v>
       </c>
       <c r="Q17" t="s">
@@ -2770,7 +2770,7 @@
       <c r="O18">
         <v>1</v>
       </c>
-      <c r="P18" s="17" t="s">
+      <c r="P18" t="s">
         <v>256</v>
       </c>
       <c r="Q18" t="s">
@@ -2826,13 +2826,13 @@
       <c r="M19" t="s">
         <v>260</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" t="s">
         <v>185</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="P19" s="17" t="s">
+      <c r="P19" t="s">
         <v>261</v>
       </c>
       <c r="Q19" t="s">
@@ -2894,7 +2894,7 @@
       <c r="O20">
         <v>1</v>
       </c>
-      <c r="P20" s="17" t="s">
+      <c r="P20" t="s">
         <v>267</v>
       </c>
       <c r="Q20" t="s">
@@ -2950,13 +2950,13 @@
       <c r="M21" t="s">
         <v>271</v>
       </c>
-      <c r="N21" s="16" t="s">
+      <c r="N21" t="s">
         <v>185</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
-      <c r="P21" s="17" t="s">
+      <c r="P21" t="s">
         <v>272</v>
       </c>
       <c r="Q21" t="s">
@@ -3012,13 +3012,13 @@
       <c r="M22" t="s">
         <v>294</v>
       </c>
-      <c r="N22" s="16" t="s">
+      <c r="N22" t="s">
         <v>185</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22" s="17" t="s">
+      <c r="P22" t="s">
         <v>296</v>
       </c>
       <c r="Q22" t="s">
@@ -3080,7 +3080,7 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="P23" s="17" t="s">
+      <c r="P23" t="s">
         <v>299</v>
       </c>
       <c r="Q23" t="s">
@@ -3136,13 +3136,13 @@
       <c r="M24" t="s">
         <v>307</v>
       </c>
-      <c r="N24" s="16" t="s">
+      <c r="N24" t="s">
         <v>185</v>
       </c>
       <c r="O24">
         <v>1</v>
       </c>
-      <c r="P24" s="17" t="s">
+      <c r="P24" t="s">
         <v>309</v>
       </c>
       <c r="Q24" t="s">
@@ -3195,7 +3195,7 @@
       <c r="L25" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="M25" s="17" t="s">
+      <c r="M25" t="s">
         <v>314</v>
       </c>
       <c r="N25" s="15" t="s">
@@ -3204,16 +3204,16 @@
       <c r="O25">
         <v>0</v>
       </c>
-      <c r="P25" s="17" t="s">
+      <c r="P25" t="s">
         <v>185</v>
       </c>
       <c r="Q25" t="s">
         <v>153</v>
       </c>
-      <c r="R25" s="17" t="s">
+      <c r="R25" t="s">
         <v>156</v>
       </c>
-      <c r="S25" s="18" t="s">
+      <c r="S25" t="s">
         <v>317</v>
       </c>
       <c r="T25" s="13" t="s">
@@ -3257,7 +3257,7 @@
       <c r="L26" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="M26" s="17" t="s">
+      <c r="M26" t="s">
         <v>319</v>
       </c>
       <c r="N26" s="15" t="s">
@@ -3266,16 +3266,16 @@
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="P26" s="17" t="s">
+      <c r="P26" t="s">
         <v>185</v>
       </c>
       <c r="Q26" t="s">
         <v>155</v>
       </c>
-      <c r="R26" s="17" t="s">
+      <c r="R26" t="s">
         <v>155</v>
       </c>
-      <c r="S26" s="18" t="s">
+      <c r="S26" t="s">
         <v>321</v>
       </c>
       <c r="T26" s="13" t="s">
@@ -3322,22 +3322,22 @@
       <c r="M27" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="N27" s="16" t="s">
+      <c r="N27" t="s">
         <v>185</v>
       </c>
       <c r="O27">
         <v>1</v>
       </c>
-      <c r="P27" s="17" t="s">
+      <c r="P27" t="s">
         <v>185</v>
       </c>
       <c r="Q27" t="s">
         <v>155</v>
       </c>
-      <c r="R27" s="17" t="s">
+      <c r="R27" t="s">
         <v>155</v>
       </c>
-      <c r="S27" s="18" t="s">
+      <c r="S27" t="s">
         <v>330</v>
       </c>
       <c r="T27" s="13" t="s">
@@ -3378,7 +3378,7 @@
       <c r="L28" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="M28" s="17" t="s">
+      <c r="M28" t="s">
         <v>333</v>
       </c>
       <c r="N28" s="15" t="s">
@@ -3387,16 +3387,16 @@
       <c r="O28">
         <v>0</v>
       </c>
-      <c r="P28" s="17" t="s">
+      <c r="P28" t="s">
         <v>343</v>
       </c>
       <c r="Q28" t="s">
         <v>155</v>
       </c>
-      <c r="R28" s="17" t="s">
+      <c r="R28" t="s">
         <v>155</v>
       </c>
-      <c r="S28" s="18" t="s">
+      <c r="S28" t="s">
         <v>342</v>
       </c>
       <c r="T28" s="13" t="s">
@@ -3438,7 +3438,7 @@
       <c r="L29" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="M29" s="17" t="s">
+      <c r="M29" t="s">
         <v>336</v>
       </c>
       <c r="N29" s="15" t="s">
@@ -3447,16 +3447,16 @@
       <c r="O29">
         <v>0</v>
       </c>
-      <c r="P29" s="17" t="s">
+      <c r="P29" t="s">
         <v>341</v>
       </c>
       <c r="Q29" t="s">
         <v>155</v>
       </c>
-      <c r="R29" s="17" t="s">
+      <c r="R29" t="s">
         <v>155</v>
       </c>
-      <c r="S29" s="18" t="s">
+      <c r="S29" t="s">
         <v>340</v>
       </c>
       <c r="T29" s="13" t="s">
@@ -3470,58 +3470,38 @@
       <c r="J30" s="1"/>
       <c r="K30" s="5"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="17"/>
       <c r="N30" s="15"/>
-      <c r="P30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
       <c r="U30" s="3"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="J31" s="1"/>
       <c r="K31" s="5"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="17"/>
       <c r="N31" s="15"/>
-      <c r="P31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
       <c r="U31" s="3"/>
     </row>
     <row r="33" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J33" s="1"/>
       <c r="K33" s="5"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="17"/>
       <c r="N33" s="15"/>
-      <c r="P33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
       <c r="U33" s="3"/>
     </row>
     <row r="34" spans="10:21" x14ac:dyDescent="0.2">
       <c r="J34" s="1"/>
       <c r="K34" s="5"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="17"/>
       <c r="N34" s="15"/>
-      <c r="P34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
       <c r="U34" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E33:E34 E3:E31">
+  <conditionalFormatting sqref="E3:E31 E33:E34">
     <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I34 I3:I31">
+  <conditionalFormatting sqref="I3:I31 I33:I34">
     <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"None"</formula>
     </cfRule>
@@ -3540,7 +3520,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N33:N34 N3:N31">
+  <conditionalFormatting sqref="N3:N31 N33:N34">
     <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
       <formula>"not specified"</formula>
     </cfRule>
@@ -3548,22 +3528,22 @@
       <formula>"not specified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O33:O34 O3:O31">
+  <conditionalFormatting sqref="O3:O31 O33:O34">
     <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q33:R34 Q3:R31">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">
-      <formula>"Not mentioned"</formula>
+  <conditionalFormatting sqref="P3:P31 P33:P34">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"not specified"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:R31 Q33:R34">
     <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"not mentioned"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P33:P34 P3:P31">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"not specified"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notEqual">
+      <formula>"Not mentioned"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -3692,7 +3672,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7254ACE7-56C6-5040-ABFE-788EED7DE7C7}">
-  <dimension ref="B2:I46"/>
+  <dimension ref="B2:I44"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D60" sqref="D60"/>
@@ -4105,7 +4085,7 @@
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="16" t="s">
+      <c r="B38" t="s">
         <v>60</v>
       </c>
       <c r="C38">
@@ -4119,7 +4099,7 @@
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="16" t="s">
+      <c r="B39" t="s">
         <v>60</v>
       </c>
       <c r="C39">
@@ -4133,7 +4113,7 @@
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="16" t="s">
+      <c r="B40" t="s">
         <v>278</v>
       </c>
       <c r="C40">
@@ -4147,7 +4127,7 @@
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="16" t="s">
+      <c r="B41" t="s">
         <v>279</v>
       </c>
       <c r="C41">
@@ -4161,7 +4141,7 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="16" t="s">
+      <c r="B42" t="s">
         <v>280</v>
       </c>
       <c r="C42">
@@ -4175,7 +4155,7 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" s="16" t="s">
+      <c r="B43" t="s">
         <v>281</v>
       </c>
       <c r="C43">
@@ -4189,7 +4169,7 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="16" t="s">
+      <c r="B44" t="s">
         <v>282</v>
       </c>
       <c r="C44">
@@ -4201,12 +4181,6 @@
       <c r="E44" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="16"/>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B46" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4680,7 +4654,7 @@
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="16" t="s">
+      <c r="B37" t="s">
         <v>282</v>
       </c>
       <c r="C37" t="s">
@@ -4693,7 +4667,7 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="16" t="s">
+      <c r="B38" t="s">
         <v>289</v>
       </c>
       <c r="C38" t="s">
@@ -4705,7 +4679,7 @@
       <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="16" t="s">
+      <c r="B39" t="s">
         <v>290</v>
       </c>
       <c r="C39" t="s">
@@ -4719,7 +4693,7 @@
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="16" t="s">
+      <c r="B40" t="s">
         <v>291</v>
       </c>
       <c r="C40" t="s">

</xml_diff>